<commit_message>
multiple cc email by excel
</commit_message>
<xml_diff>
--- a/assets/templates/DEBITNOTE_TEMPLATE.xlsx
+++ b/assets/templates/DEBITNOTE_TEMPLATE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rybzki\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp7\htdocs\ut-dev\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1ED3FE4-CF3D-453D-B2AB-C114414E63B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E5B22-46CA-4803-BE8E-ECD0444084AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C72F07B6-0C7C-4935-8A48-F30E0F5F96DB}"/>
+    <workbookView xWindow="4470" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{C72F07B6-0C7C-4935-8A48-F30E0F5F96DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>DEBIT NOTE</t>
   </si>
@@ -132,34 +132,10 @@
     <t>TAGIHAN ATAS 3 UNIT GENOSE</t>
   </si>
   <si>
-    <t>010.002-21,18888013</t>
-  </si>
-  <si>
-    <t>TAGIHAN PEMAKAIAN TELEPON FEBRUARI 2021</t>
-  </si>
-  <si>
-    <t>010.002-21-18888007</t>
-  </si>
-  <si>
-    <t>PT ATMC PUMP SERVICES</t>
-  </si>
-  <si>
-    <t>ACSET BUILDING JL. MAJAPAHIT - PETOJO SELATAN GAMBIR JAKARTA PUSAT DKI JAKARTA</t>
-  </si>
-  <si>
-    <t>71.017.856.7-028.000</t>
-  </si>
-  <si>
-    <t>TAGIHAN PEMAKAIAN LISTRIK FEBRUARI 2021</t>
-  </si>
-  <si>
-    <t>komatsu@gmail.com</t>
-  </si>
-  <si>
     <t>pamapersada@gmail.com</t>
   </si>
   <si>
-    <t>atmc@gmail.com</t>
+    <t>komatsu@gmail.com;atmc@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -169,7 +145,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -282,7 +258,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -607,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B535AA9-1850-4F2C-B2B5-85AA3E2B2631}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +773,7 @@
         <v>23157</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>24</v>
@@ -867,7 +843,7 @@
         <v>10611</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>24</v>
@@ -915,225 +891,12 @@
       <c r="V6" s="7">
         <f>SUM(T6:U6)</f>
         <v>204600000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>1610000442</v>
-      </c>
-      <c r="B7" s="6">
-        <v>44273</v>
-      </c>
-      <c r="C7" s="6">
-        <v>44304</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="5">
-        <v>190</v>
-      </c>
-      <c r="F7" s="5">
-        <v>23157</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="6">
-        <v>44273</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O7" s="7">
-        <v>1131215</v>
-      </c>
-      <c r="P7" s="7">
-        <v>1131215</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>0</v>
-      </c>
-      <c r="R7" s="7">
-        <v>0</v>
-      </c>
-      <c r="S7" s="7">
-        <v>0</v>
-      </c>
-      <c r="T7" s="7">
-        <v>1131215</v>
-      </c>
-      <c r="U7" s="7">
-        <f>T7*0.1</f>
-        <v>113121.5</v>
-      </c>
-      <c r="V7" s="7">
-        <f>SUM(T7:U7)</f>
-        <v>1244336.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>1610000436</v>
-      </c>
-      <c r="B8" s="6">
-        <v>44273</v>
-      </c>
-      <c r="C8" s="6">
-        <v>44304</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5">
-        <v>35154</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="6">
-        <v>44273</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="7">
-        <v>1121983</v>
-      </c>
-      <c r="P8" s="7">
-        <v>1121983</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>0</v>
-      </c>
-      <c r="R8" s="7">
-        <v>0</v>
-      </c>
-      <c r="S8" s="7">
-        <v>0</v>
-      </c>
-      <c r="T8" s="7">
-        <v>1121983</v>
-      </c>
-      <c r="U8" s="7">
-        <f>T8*0.1</f>
-        <v>112198.3</v>
-      </c>
-      <c r="V8" s="7">
-        <f>SUM(T8:U8)</f>
-        <v>1234181.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>1610000436</v>
-      </c>
-      <c r="B9" s="6">
-        <v>44273</v>
-      </c>
-      <c r="C9" s="6">
-        <v>44305</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="5">
-        <v>35154</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="6">
-        <v>44273</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="7">
-        <v>1121983</v>
-      </c>
-      <c r="P9" s="7">
-        <v>1121983</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>0</v>
-      </c>
-      <c r="R9" s="7">
-        <v>0</v>
-      </c>
-      <c r="S9" s="7">
-        <v>0</v>
-      </c>
-      <c r="T9" s="7">
-        <v>1121983</v>
-      </c>
-      <c r="U9" s="7">
-        <f>T9*0.1</f>
-        <v>112198.3</v>
-      </c>
-      <c r="V9" s="7">
-        <f>SUM(T9:U9)</f>
-        <v>1234181.3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{AAF272EF-A64D-4365-8915-3E74392A6F45}"/>
     <hyperlink ref="G6" r:id="rId2" xr:uid="{D7EA46B4-26BD-4FAD-8865-3B05031F3B0A}"/>
-    <hyperlink ref="G7" r:id="rId3" xr:uid="{8A98801A-7792-4B78-B1EC-65B45D558244}"/>
-    <hyperlink ref="G8" r:id="rId4" xr:uid="{573EDFE3-B18D-4C68-A5DD-06B96D52C1D1}"/>
-    <hyperlink ref="G9" r:id="rId5" xr:uid="{24D5DA29-00A6-450A-80EC-29EBE2B1DB83}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dn template add typedn
</commit_message>
<xml_diff>
--- a/assets/templates/DEBITNOTE_TEMPLATE.xlsx
+++ b/assets/templates/DEBITNOTE_TEMPLATE.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp7\htdocs\ut-dev\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giriel\Documents\GitHub\ut-dev\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E5B22-46CA-4803-BE8E-ECD0444084AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{C72F07B6-0C7C-4935-8A48-F30E0F5F96DB}"/>
+    <workbookView xWindow="4470" yWindow="3150" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tipe" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>DEBIT NOTE</t>
   </si>
@@ -136,12 +136,24 @@
   </si>
   <si>
     <t>komatsu@gmail.com;atmc@gmail.com</t>
+  </si>
+  <si>
+    <t>Listrik</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Tipe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
@@ -209,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -232,13 +244,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -267,6 +290,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -582,11 +609,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B535AA9-1850-4F2C-B2B5-85AA3E2B2631}">
-  <dimension ref="A1:V6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +638,7 @@
     <col min="22" max="22" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +664,7 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -661,7 +688,7 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -685,7 +712,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -752,8 +779,11 @@
       <c r="V4" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="W4" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1610001597</v>
       </c>
@@ -822,8 +852,11 @@
         <f>SUM(T5:U5)</f>
         <v>247623750</v>
       </c>
+      <c r="W5" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1610000576</v>
       </c>
@@ -892,12 +925,57 @@
         <f>SUM(T6:U6)</f>
         <v>204600000</v>
       </c>
+      <c r="W6" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{AAF272EF-A64D-4365-8915-3E74392A6F45}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{D7EA46B4-26BD-4FAD-8865-3B05031F3B0A}"/>
+    <hyperlink ref="G5" r:id="rId1"/>
+    <hyperlink ref="G6" r:id="rId2"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Tipe!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>W5:W6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tipe dn excel, RnO, APR
</commit_message>
<xml_diff>
--- a/assets/templates/DEBITNOTE_TEMPLATE.xlsx
+++ b/assets/templates/DEBITNOTE_TEMPLATE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>DEBIT NOTE</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>Tipe</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -613,7 +622,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +949,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Tipe!$B$2:$B$4</xm:f>
+            <xm:f>Tipe!$B$2:$B$7</xm:f>
           </x14:formula1>
           <xm:sqref>W5:W6</xm:sqref>
         </x14:dataValidation>
@@ -952,10 +961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,6 +984,21 @@
         <v>39</v>
       </c>
     </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>